<commit_message>
Deal with Radar wierdness
</commit_message>
<xml_diff>
--- a/Cornell-VMIT-Tech-Radar.xlsx
+++ b/Cornell-VMIT-Tech-Radar.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cr396/src/cuvmit-tech-radar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C77BC1DA-ABD3-D24B-A8CD-D912DF8FDCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7DB8AE-C4A2-B745-B850-787D0046B18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="6660" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="28560" yWindow="6680" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cornell-VMIT-Tech-Radar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -173,12 +173,18 @@
   </si>
   <si>
     <t>Run automated tests and use as gatekeeper for deployment</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>Angular is a client-based SPA Framework.  I'm listing it here because the Radar draws the rings in order listed in the spreadsheet, wierdly.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1012,11 +1018,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1045,10 +1051,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1057,12 +1063,12 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1074,12 +1080,12 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1091,12 +1097,12 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -1108,15 +1114,15 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1125,12 +1131,12 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1142,12 +1148,12 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1159,32 +1165,32 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -1193,15 +1199,15 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1210,29 +1216,29 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -1244,12 +1250,12 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1261,29 +1267,29 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -1295,12 +1301,12 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -1312,12 +1318,12 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -1329,15 +1335,15 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
@@ -1346,12 +1352,12 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -1363,6 +1369,23 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>